<commit_message>
[#89] test: Add dependency value checks in FakeCompleteDataSeederTestCase and update example forms
</commit_message>
<xml_diff>
--- a/backend/api/v1/v1_jobs/tests/fixtures/test-error-multi-dependency.xlsx
+++ b/backend/api/v1/v1_jobs/tests/fixtures/test-error-multi-dependency.xlsx
@@ -8,9 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="questions" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="options" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="data" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="questions" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="options" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -200,7 +200,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -230,12 +230,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -292,23 +286,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -324,20 +318,126 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2:O2"/>
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -397,7 +497,7 @@
       <c r="I2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="K2" s="2" t="s">
@@ -417,7 +517,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G6" s="3"/>
+      <c r="G6" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -431,19 +531,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="M2:O2 A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="26.24"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -467,89 +567,89 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -570,17 +670,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="M2:O2 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -594,79 +694,79 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="3" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>